<commit_message>
All API calls added
</commit_message>
<xml_diff>
--- a/Traditional Yoga Updated Document.xlsx
+++ b/Traditional Yoga Updated Document.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Traditional Yoga\TY Excelsheet\yoga_excelsheet\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976E99C3-65DF-4EA8-900B-27FAEC0F19AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="5" r:id="rId1"/>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2906" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2909" uniqueCount="392">
   <si>
     <t xml:space="preserve">Module </t>
   </si>
@@ -1211,7 +1205,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1917,7 +1911,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1927,45 +1941,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1980,6 +1955,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1989,20 +1988,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2330,14 +2324,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2448,12 +2442,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="B2:K349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:E50"/>
+    <sheetView tabSelected="1" topLeftCell="B51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,7 +2617,7 @@
       </c>
       <c r="K6" s="62"/>
     </row>
-    <row r="7" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="72">
         <v>3</v>
       </c>
@@ -2653,7 +2647,7 @@
       </c>
       <c r="K7" s="72"/>
     </row>
-    <row r="8" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="72">
         <v>5</v>
       </c>
@@ -2743,7 +2737,7 @@
       </c>
       <c r="K10" s="72"/>
     </row>
-    <row r="11" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="72">
         <v>7</v>
       </c>
@@ -2773,7 +2767,7 @@
       </c>
       <c r="K11" s="72"/>
     </row>
-    <row r="12" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="72">
         <v>9</v>
       </c>
@@ -2863,7 +2857,7 @@
       </c>
       <c r="K14" s="72"/>
     </row>
-    <row r="15" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="72">
         <v>11</v>
       </c>
@@ -2893,7 +2887,7 @@
       </c>
       <c r="K15" s="72"/>
     </row>
-    <row r="16" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="72">
         <v>13</v>
       </c>
@@ -2923,7 +2917,7 @@
       </c>
       <c r="K16" s="72"/>
     </row>
-    <row r="17" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="72">
         <v>15</v>
       </c>
@@ -2953,7 +2947,7 @@
       </c>
       <c r="K17" s="72"/>
     </row>
-    <row r="18" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="72">
         <v>17</v>
       </c>
@@ -2983,127 +2977,127 @@
       </c>
       <c r="K18" s="72"/>
     </row>
-    <row r="19" spans="2:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="99">
+    <row r="19" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="75">
         <v>22</v>
       </c>
-      <c r="C19" s="99" t="s">
+      <c r="C19" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="99" t="s">
+      <c r="D19" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="99" t="s">
+      <c r="E19" s="75" t="s">
         <v>374</v>
       </c>
-      <c r="F19" s="99" t="s">
+      <c r="F19" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="G19" s="99" t="s">
+      <c r="G19" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="H19" s="100">
+      <c r="H19" s="76">
         <v>44881</v>
       </c>
-      <c r="I19" s="100">
+      <c r="I19" s="76">
         <v>44872</v>
       </c>
-      <c r="J19" s="99" t="s">
+      <c r="J19" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="K19" s="99"/>
-    </row>
-    <row r="20" spans="2:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="99">
+      <c r="K19" s="75"/>
+    </row>
+    <row r="20" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="75">
         <v>24</v>
       </c>
-      <c r="C20" s="99" t="s">
+      <c r="C20" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="99" t="s">
+      <c r="D20" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="99" t="s">
+      <c r="E20" s="75" t="s">
         <v>374</v>
       </c>
-      <c r="F20" s="99" t="s">
+      <c r="F20" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="G20" s="99" t="s">
+      <c r="G20" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="H20" s="100">
+      <c r="H20" s="76">
         <v>44881</v>
       </c>
-      <c r="I20" s="100">
+      <c r="I20" s="76">
         <v>44872</v>
       </c>
-      <c r="J20" s="99" t="s">
+      <c r="J20" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="K20" s="99"/>
-    </row>
-    <row r="21" spans="2:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="99">
+      <c r="K20" s="75"/>
+    </row>
+    <row r="21" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="75">
         <v>26</v>
       </c>
-      <c r="C21" s="99" t="s">
+      <c r="C21" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="99" t="s">
+      <c r="D21" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="99" t="s">
+      <c r="E21" s="75" t="s">
         <v>375</v>
       </c>
-      <c r="F21" s="99" t="s">
+      <c r="F21" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="G21" s="99" t="s">
+      <c r="G21" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="H21" s="100">
+      <c r="H21" s="76">
         <v>44881</v>
       </c>
-      <c r="I21" s="100">
+      <c r="I21" s="76">
         <v>44873</v>
       </c>
-      <c r="J21" s="99" t="s">
+      <c r="J21" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="K21" s="99"/>
-    </row>
-    <row r="22" spans="2:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="99">
+      <c r="K21" s="75"/>
+    </row>
+    <row r="22" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="75">
         <v>28</v>
       </c>
-      <c r="C22" s="99" t="s">
+      <c r="C22" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="99" t="s">
+      <c r="D22" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="99" t="s">
+      <c r="E22" s="75" t="s">
         <v>375</v>
       </c>
-      <c r="F22" s="99" t="s">
+      <c r="F22" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="G22" s="99" t="s">
+      <c r="G22" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="H22" s="100">
+      <c r="H22" s="76">
         <v>44881</v>
       </c>
-      <c r="I22" s="100">
+      <c r="I22" s="76">
         <v>44873</v>
       </c>
-      <c r="J22" s="99" t="s">
+      <c r="J22" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="K22" s="99"/>
-    </row>
-    <row r="23" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="75"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="72">
         <v>23</v>
       </c>
@@ -3133,65 +3127,65 @@
       </c>
       <c r="K23" s="72"/>
     </row>
-    <row r="24" spans="2:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="99">
+    <row r="24" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="75">
         <v>30</v>
       </c>
-      <c r="C24" s="99" t="s">
+      <c r="C24" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="102" t="s">
+      <c r="D24" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="99" t="s">
+      <c r="E24" s="75" t="s">
         <v>374</v>
       </c>
-      <c r="F24" s="99" t="s">
+      <c r="F24" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="G24" s="99" t="s">
-        <v>166</v>
-      </c>
-      <c r="H24" s="100">
+      <c r="G24" s="75" t="s">
+        <v>381</v>
+      </c>
+      <c r="H24" s="76">
         <v>44881</v>
       </c>
-      <c r="I24" s="100">
+      <c r="I24" s="76">
         <v>44874</v>
       </c>
-      <c r="J24" s="99" t="s">
+      <c r="J24" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="K24" s="99"/>
-    </row>
-    <row r="25" spans="2:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="99">
+      <c r="K24" s="75"/>
+    </row>
+    <row r="25" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="75">
         <v>32</v>
       </c>
-      <c r="C25" s="99" t="s">
+      <c r="C25" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="99" t="s">
+      <c r="D25" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="99" t="s">
+      <c r="E25" s="75" t="s">
         <v>374</v>
       </c>
-      <c r="F25" s="99" t="s">
+      <c r="F25" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="G25" s="99" t="s">
+      <c r="G25" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="H25" s="100">
+      <c r="H25" s="76">
         <v>44881</v>
       </c>
-      <c r="I25" s="100">
+      <c r="I25" s="76">
         <v>44874</v>
       </c>
-      <c r="J25" s="99" t="s">
+      <c r="J25" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="K25" s="99"/>
+      <c r="K25" s="75"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="63">
@@ -3217,7 +3211,7 @@
       <c r="J26" s="63"/>
       <c r="K26" s="63"/>
     </row>
-    <row r="27" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="72">
         <v>27</v>
       </c>
@@ -3247,7 +3241,7 @@
       </c>
       <c r="K27" s="72"/>
     </row>
-    <row r="28" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="72">
         <v>29</v>
       </c>
@@ -3277,67 +3271,67 @@
       </c>
       <c r="K28" s="72"/>
     </row>
-    <row r="29" spans="2:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="99">
+    <row r="29" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="75">
         <v>34</v>
       </c>
-      <c r="C29" s="99" t="s">
+      <c r="C29" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="102" t="s">
+      <c r="D29" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="99" t="s">
+      <c r="E29" s="75" t="s">
         <v>375</v>
       </c>
-      <c r="F29" s="99" t="s">
+      <c r="F29" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="G29" s="99" t="s">
+      <c r="G29" s="75" t="s">
+        <v>381</v>
+      </c>
+      <c r="H29" s="76">
+        <v>44881</v>
+      </c>
+      <c r="I29" s="76">
+        <v>44875</v>
+      </c>
+      <c r="J29" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="K29" s="75"/>
+    </row>
+    <row r="30" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="75">
+        <v>36</v>
+      </c>
+      <c r="C30" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="75" t="s">
+        <v>374</v>
+      </c>
+      <c r="F30" s="75" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="H29" s="100">
+      <c r="H30" s="76">
         <v>44881</v>
       </c>
-      <c r="I29" s="100">
+      <c r="I30" s="76">
         <v>44875</v>
       </c>
-      <c r="J29" s="99" t="s">
-        <v>157</v>
-      </c>
-      <c r="K29" s="99"/>
-    </row>
-    <row r="30" spans="2:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="99">
-        <v>36</v>
-      </c>
-      <c r="C30" s="99" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="102" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="99" t="s">
-        <v>374</v>
-      </c>
-      <c r="F30" s="99" t="s">
-        <v>152</v>
-      </c>
-      <c r="G30" s="99" t="s">
-        <v>166</v>
-      </c>
-      <c r="H30" s="100">
-        <v>44881</v>
-      </c>
-      <c r="I30" s="100">
-        <v>44875</v>
-      </c>
-      <c r="J30" s="99" t="s">
+      <c r="J30" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="K30" s="99"/>
-    </row>
-    <row r="31" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="75"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>37</v>
       </c>
@@ -3353,7 +3347,7 @@
       <c r="F31" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G31" s="98" t="s">
+      <c r="G31" s="74" t="s">
         <v>381</v>
       </c>
       <c r="H31" s="69">
@@ -3369,7 +3363,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="32" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>25</v>
       </c>
@@ -3399,7 +3393,7 @@
       </c>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="72">
         <v>31</v>
       </c>
@@ -3429,7 +3423,7 @@
       </c>
       <c r="K33" s="72"/>
     </row>
-    <row r="34" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="72">
         <v>33</v>
       </c>
@@ -3459,7 +3453,7 @@
       </c>
       <c r="K34" s="72"/>
     </row>
-    <row r="35" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="72">
         <v>35</v>
       </c>
@@ -3489,78 +3483,78 @@
       </c>
       <c r="K35" s="72"/>
     </row>
-    <row r="36" spans="2:11" s="101" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="99">
+    <row r="36" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="75">
         <v>39</v>
       </c>
-      <c r="C36" s="99" t="s">
+      <c r="C36" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="99" t="s">
+      <c r="D36" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="99" t="s">
+      <c r="E36" s="75" t="s">
         <v>371</v>
       </c>
-      <c r="F36" s="99" t="s">
+      <c r="F36" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="G36" s="99" t="s">
+      <c r="G36" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="H36" s="100">
+      <c r="H36" s="76">
         <v>44880</v>
       </c>
-      <c r="I36" s="100">
+      <c r="I36" s="76">
         <v>44881</v>
       </c>
-      <c r="J36" s="99" t="s">
+      <c r="J36" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="K36" s="99" t="s">
+      <c r="K36" s="75" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="37" spans="2:11" s="101" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="99">
+    <row r="37" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="75">
         <v>41</v>
       </c>
-      <c r="C37" s="99" t="s">
+      <c r="C37" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="99" t="s">
+      <c r="D37" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="99" t="s">
+      <c r="E37" s="75" t="s">
         <v>371</v>
       </c>
-      <c r="F37" s="99" t="s">
+      <c r="F37" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="G37" s="99" t="s">
+      <c r="G37" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="H37" s="100">
+      <c r="H37" s="76">
         <v>44880</v>
       </c>
-      <c r="I37" s="100">
+      <c r="I37" s="76">
         <v>44881</v>
       </c>
-      <c r="J37" s="99" t="s">
+      <c r="J37" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="K37" s="99" t="s">
+      <c r="K37" s="75" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="38" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="72">
         <v>43</v>
       </c>
       <c r="C38" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="103" t="s">
+      <c r="D38" s="79" t="s">
         <v>16</v>
       </c>
       <c r="E38" s="72" t="s">
@@ -3569,7 +3563,7 @@
       <c r="F38" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="G38" s="98" t="s">
+      <c r="G38" s="74" t="s">
         <v>381</v>
       </c>
       <c r="H38" s="73">
@@ -3590,7 +3584,7 @@
       <c r="C39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="102" t="s">
+      <c r="D39" s="78" t="s">
         <v>13</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -3650,7 +3644,7 @@
       <c r="C41" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="102" t="s">
+      <c r="D41" s="78" t="s">
         <v>15</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -3660,7 +3654,7 @@
         <v>152</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>166</v>
+        <v>381</v>
       </c>
       <c r="H41" s="64">
         <v>44879</v>
@@ -3680,7 +3674,7 @@
       <c r="C42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="102" t="s">
+      <c r="D42" s="78" t="s">
         <v>16</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -3690,7 +3684,7 @@
         <v>152</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>383</v>
+        <v>166</v>
       </c>
       <c r="H42" s="64">
         <v>44879</v>
@@ -3703,7 +3697,7 @@
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="72">
         <v>45</v>
       </c>
@@ -3733,67 +3727,67 @@
       </c>
       <c r="K43" s="72"/>
     </row>
-    <row r="44" spans="2:11" s="101" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="99">
+    <row r="44" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="75">
         <v>47</v>
       </c>
-      <c r="C44" s="99" t="s">
+      <c r="C44" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D44" s="99" t="s">
+      <c r="D44" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="E44" s="99" t="s">
+      <c r="E44" s="75" t="s">
         <v>371</v>
       </c>
-      <c r="F44" s="99" t="s">
+      <c r="F44" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="G44" s="99" t="s">
+      <c r="G44" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="H44" s="100">
+      <c r="H44" s="76">
         <v>44882</v>
       </c>
-      <c r="I44" s="100">
+      <c r="I44" s="76">
         <v>44882</v>
       </c>
-      <c r="J44" s="99" t="s">
+      <c r="J44" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="K44" s="99" t="s">
+      <c r="K44" s="75" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="45" spans="2:11" s="101" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="99">
+    <row r="45" spans="2:11" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="75">
         <v>49</v>
       </c>
-      <c r="C45" s="99" t="s">
+      <c r="C45" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D45" s="99" t="s">
+      <c r="D45" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="99" t="s">
+      <c r="E45" s="75" t="s">
         <v>371</v>
       </c>
-      <c r="F45" s="99" t="s">
+      <c r="F45" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="G45" s="99" t="s">
+      <c r="G45" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="H45" s="100">
+      <c r="H45" s="76">
         <v>44882</v>
       </c>
-      <c r="I45" s="100">
+      <c r="I45" s="76">
         <v>44882</v>
       </c>
-      <c r="J45" s="99" t="s">
+      <c r="J45" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="K45" s="99" t="s">
+      <c r="K45" s="75" t="s">
         <v>379</v>
       </c>
     </row>
@@ -3804,7 +3798,7 @@
       <c r="C46" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="102" t="s">
+      <c r="D46" s="78" t="s">
         <v>17</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -3814,7 +3808,7 @@
         <v>152</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>166</v>
+        <v>381</v>
       </c>
       <c r="H46" s="64">
         <v>44880</v>
@@ -3836,7 +3830,7 @@
       <c r="C47" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="102" t="s">
+      <c r="D47" s="78" t="s">
         <v>18</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -3866,7 +3860,7 @@
       <c r="C48" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="102" t="s">
+      <c r="D48" s="78" t="s">
         <v>19</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -3889,7 +3883,7 @@
       </c>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="72">
         <v>51</v>
       </c>
@@ -3926,7 +3920,7 @@
       <c r="C50" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="102" t="s">
+      <c r="D50" s="78" t="s">
         <v>20</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -3949,7 +3943,7 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="72">
         <v>53</v>
       </c>
@@ -3986,7 +3980,7 @@
       <c r="C52" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="102" t="s">
+      <c r="D52" s="78" t="s">
         <v>21</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -4009,7 +4003,7 @@
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>55</v>
       </c>
@@ -4046,7 +4040,7 @@
       <c r="C54" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D54" s="102" t="s">
+      <c r="D54" s="78" t="s">
         <v>22</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -4069,7 +4063,7 @@
       </c>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="72">
         <v>57</v>
       </c>
@@ -4243,7 +4237,7 @@
       </c>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="72">
         <v>59</v>
       </c>
@@ -4273,7 +4267,7 @@
       </c>
       <c r="K61" s="72"/>
     </row>
-    <row r="62" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="4">
         <v>61</v>
       </c>
@@ -4359,7 +4353,7 @@
       </c>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="4">
         <v>63</v>
       </c>
@@ -4389,7 +4383,7 @@
       </c>
       <c r="K65" s="4"/>
     </row>
-    <row r="66" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" s="1">
         <v>65</v>
       </c>
@@ -4399,12 +4393,14 @@
       <c r="D66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E66" s="1"/>
+      <c r="E66" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="F66" s="1" t="s">
         <v>161</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>383</v>
+        <v>166</v>
       </c>
       <c r="H66" s="64">
         <v>44888</v>
@@ -4417,7 +4413,7 @@
       </c>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" s="1">
         <v>72</v>
       </c>
@@ -4445,7 +4441,7 @@
       </c>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>74</v>
       </c>
@@ -4473,7 +4469,7 @@
       </c>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>67</v>
       </c>
@@ -4483,12 +4479,14 @@
       <c r="D69" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E69" s="1"/>
+      <c r="E69" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="F69" s="1" t="s">
         <v>161</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>383</v>
+        <v>166</v>
       </c>
       <c r="H69" s="64">
         <v>44889</v>
@@ -4501,7 +4499,7 @@
       </c>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" s="1">
         <v>69</v>
       </c>
@@ -4511,12 +4509,14 @@
       <c r="D70" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E70" s="1"/>
+      <c r="E70" s="1" t="s">
+        <v>371</v>
+      </c>
       <c r="F70" s="1" t="s">
         <v>161</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>383</v>
+        <v>166</v>
       </c>
       <c r="H70" s="64">
         <v>44889</v>
@@ -4529,7 +4529,7 @@
       </c>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>76</v>
       </c>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="1">
         <v>78</v>
       </c>
@@ -12173,7 +12173,7 @@
       </c>
       <c r="K343" s="1"/>
     </row>
-    <row r="344" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B344" s="63">
         <v>18</v>
       </c>
@@ -12225,7 +12225,7 @@
       </c>
       <c r="K345" s="63"/>
     </row>
-    <row r="346" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B346" s="1">
         <v>343</v>
       </c>
@@ -12245,7 +12245,7 @@
       <c r="J346" s="1"/>
       <c r="K346" s="1"/>
     </row>
-    <row r="347" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B347" s="1">
         <v>344</v>
       </c>
@@ -12265,7 +12265,7 @@
       <c r="J347" s="1"/>
       <c r="K347" s="1"/>
     </row>
-    <row r="348" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B348" s="1">
         <v>345</v>
       </c>
@@ -12285,7 +12285,7 @@
       <c r="J348" s="1"/>
       <c r="K348" s="1"/>
     </row>
-    <row r="349" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B349" s="1">
         <v>346</v>
       </c>
@@ -12306,34 +12306,30 @@
       <c r="K349" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:K349" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <filterColumn colId="4">
-      <filters blank="1">
-        <filter val="API"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters blank="1">
+  <autoFilter ref="B2:K349">
+    <filterColumn colId="7">
+      <filters>
         <dateGroupItem year="2022" month="10" dateTimeGrouping="month"/>
         <dateGroupItem year="2022" month="11" day="1" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="2" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="3" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="4" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="7" dateTimeGrouping="day"/>
+        <dateGroupItem year="2022" month="11" day="8" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="9" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="10" dateTimeGrouping="day"/>
-        <dateGroupItem year="2022" month="11" day="11" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="14" dateTimeGrouping="day"/>
-        <dateGroupItem year="2022" month="11" day="15" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="16" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="17" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="18" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="21" dateTimeGrouping="day"/>
         <dateGroupItem year="2022" month="11" day="22" dateTimeGrouping="day"/>
+        <dateGroupItem year="2022" month="11" day="23" dateTimeGrouping="day"/>
+        <dateGroupItem year="2022" month="11" day="24" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:K349">
+  <sortState ref="B3:K349">
     <sortCondition ref="I2"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -12349,7 +12345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q320"/>
   <sheetViews>
     <sheetView topLeftCell="A301" zoomScaleNormal="100" workbookViewId="0">
@@ -12365,15 +12361,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
@@ -12441,14 +12437,14 @@
       <c r="H4" s="44">
         <v>55</v>
       </c>
-      <c r="J4" s="92" t="s">
+      <c r="J4" s="87" t="s">
         <v>211</v>
       </c>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="94"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="89"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="39">
@@ -12565,15 +12561,15 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="90" t="s">
         <v>212</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="87"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="92"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
@@ -12725,14 +12721,14 @@
       <c r="H19" s="3">
         <v>10</v>
       </c>
-      <c r="J19" s="82" t="s">
+      <c r="J19" s="93" t="s">
         <v>219</v>
       </c>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
+      <c r="K19" s="94"/>
+      <c r="L19" s="94"/>
+      <c r="M19" s="94"/>
+      <c r="N19" s="94"/>
+      <c r="O19" s="95"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
@@ -12867,15 +12863,15 @@
     </row>
     <row r="25" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="90" t="s">
         <v>221</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="87"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="91"/>
+      <c r="H26" s="92"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
@@ -12964,14 +12960,14 @@
       <c r="H30" s="3">
         <v>255</v>
       </c>
-      <c r="J30" s="82" t="s">
+      <c r="J30" s="93" t="s">
         <v>225</v>
       </c>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="79"/>
-      <c r="N30" s="79"/>
-      <c r="O30" s="80"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="94"/>
+      <c r="M30" s="94"/>
+      <c r="N30" s="94"/>
+      <c r="O30" s="95"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
@@ -13035,14 +13031,14 @@
       <c r="H33" s="3">
         <v>10</v>
       </c>
-      <c r="J33" s="82" t="s">
+      <c r="J33" s="93" t="s">
         <v>219</v>
       </c>
-      <c r="K33" s="79"/>
-      <c r="L33" s="79"/>
-      <c r="M33" s="79"/>
-      <c r="N33" s="79"/>
-      <c r="O33" s="80"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="94"/>
+      <c r="O33" s="95"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
@@ -13171,15 +13167,15 @@
     </row>
     <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="95" t="s">
+      <c r="B42" s="98" t="s">
         <v>226</v>
       </c>
-      <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="96"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="97"/>
+      <c r="C42" s="99"/>
+      <c r="D42" s="99"/>
+      <c r="E42" s="99"/>
+      <c r="F42" s="99"/>
+      <c r="G42" s="99"/>
+      <c r="H42" s="100"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="27" t="s">
@@ -13349,15 +13345,15 @@
     </row>
     <row r="52" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="85" t="s">
+      <c r="B53" s="90" t="s">
         <v>229</v>
       </c>
-      <c r="C53" s="86"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
-      <c r="H53" s="87"/>
+      <c r="C53" s="91"/>
+      <c r="D53" s="91"/>
+      <c r="E53" s="91"/>
+      <c r="F53" s="91"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="92"/>
     </row>
     <row r="54" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="22" t="s">
@@ -13522,15 +13518,15 @@
     </row>
     <row r="64" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="85" t="s">
+      <c r="B65" s="90" t="s">
         <v>233</v>
       </c>
-      <c r="C65" s="86"/>
-      <c r="D65" s="86"/>
-      <c r="E65" s="86"/>
-      <c r="F65" s="86"/>
-      <c r="G65" s="86"/>
-      <c r="H65" s="87"/>
+      <c r="C65" s="91"/>
+      <c r="D65" s="91"/>
+      <c r="E65" s="91"/>
+      <c r="F65" s="91"/>
+      <c r="G65" s="91"/>
+      <c r="H65" s="92"/>
     </row>
     <row r="66" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B66" s="27" t="s">
@@ -13613,15 +13609,15 @@
         <v>188</v>
       </c>
       <c r="H69" s="3"/>
-      <c r="J69" s="82" t="s">
+      <c r="J69" s="93" t="s">
         <v>237</v>
       </c>
-      <c r="K69" s="83"/>
-      <c r="L69" s="83"/>
-      <c r="M69" s="83"/>
-      <c r="N69" s="83"/>
-      <c r="O69" s="83"/>
-      <c r="P69" s="84"/>
+      <c r="K69" s="96"/>
+      <c r="L69" s="96"/>
+      <c r="M69" s="96"/>
+      <c r="N69" s="96"/>
+      <c r="O69" s="96"/>
+      <c r="P69" s="97"/>
     </row>
     <row r="70" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B70" s="34"/>
@@ -13736,15 +13732,15 @@
     </row>
     <row r="75" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="76" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="75" t="s">
+      <c r="B76" s="83" t="s">
         <v>238</v>
       </c>
-      <c r="C76" s="76"/>
-      <c r="D76" s="76"/>
-      <c r="E76" s="76"/>
-      <c r="F76" s="76"/>
-      <c r="G76" s="76"/>
-      <c r="H76" s="77"/>
+      <c r="C76" s="84"/>
+      <c r="D76" s="84"/>
+      <c r="E76" s="84"/>
+      <c r="F76" s="84"/>
+      <c r="G76" s="84"/>
+      <c r="H76" s="85"/>
     </row>
     <row r="77" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="22" t="s">
@@ -13960,15 +13956,15 @@
     </row>
     <row r="89" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="90" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="88" t="s">
+      <c r="B90" s="80" t="s">
         <v>241</v>
       </c>
-      <c r="C90" s="89"/>
-      <c r="D90" s="89"/>
-      <c r="E90" s="89"/>
-      <c r="F90" s="89"/>
-      <c r="G90" s="89"/>
-      <c r="H90" s="90"/>
+      <c r="C90" s="81"/>
+      <c r="D90" s="81"/>
+      <c r="E90" s="81"/>
+      <c r="F90" s="81"/>
+      <c r="G90" s="81"/>
+      <c r="H90" s="82"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="31" t="s">
@@ -14224,15 +14220,15 @@
     </row>
     <row r="105" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="106" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="75" t="s">
+      <c r="B106" s="83" t="s">
         <v>247</v>
       </c>
-      <c r="C106" s="76"/>
-      <c r="D106" s="76"/>
-      <c r="E106" s="76"/>
-      <c r="F106" s="76"/>
-      <c r="G106" s="76"/>
-      <c r="H106" s="77"/>
+      <c r="C106" s="84"/>
+      <c r="D106" s="84"/>
+      <c r="E106" s="84"/>
+      <c r="F106" s="84"/>
+      <c r="G106" s="84"/>
+      <c r="H106" s="85"/>
     </row>
     <row r="107" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="49" t="s">
@@ -14494,15 +14490,15 @@
     </row>
     <row r="119" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="120" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="75" t="s">
+      <c r="B120" s="83" t="s">
         <v>259</v>
       </c>
-      <c r="C120" s="76"/>
-      <c r="D120" s="76"/>
-      <c r="E120" s="76"/>
-      <c r="F120" s="76"/>
-      <c r="G120" s="76"/>
-      <c r="H120" s="77"/>
+      <c r="C120" s="84"/>
+      <c r="D120" s="84"/>
+      <c r="E120" s="84"/>
+      <c r="F120" s="84"/>
+      <c r="G120" s="84"/>
+      <c r="H120" s="85"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="27" t="s">
@@ -14682,15 +14678,15 @@
     </row>
     <row r="132" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="133" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="75" t="s">
+      <c r="B133" s="83" t="s">
         <v>261</v>
       </c>
-      <c r="C133" s="76"/>
-      <c r="D133" s="76"/>
-      <c r="E133" s="76"/>
-      <c r="F133" s="76"/>
-      <c r="G133" s="76"/>
-      <c r="H133" s="77"/>
+      <c r="C133" s="84"/>
+      <c r="D133" s="84"/>
+      <c r="E133" s="84"/>
+      <c r="F133" s="84"/>
+      <c r="G133" s="84"/>
+      <c r="H133" s="85"/>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" s="32" t="s">
@@ -14862,15 +14858,15 @@
     </row>
     <row r="143" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="144" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="75" t="s">
+      <c r="B144" s="83" t="s">
         <v>264</v>
       </c>
-      <c r="C144" s="76"/>
-      <c r="D144" s="76"/>
-      <c r="E144" s="76"/>
-      <c r="F144" s="76"/>
-      <c r="G144" s="76"/>
-      <c r="H144" s="77"/>
+      <c r="C144" s="84"/>
+      <c r="D144" s="84"/>
+      <c r="E144" s="84"/>
+      <c r="F144" s="84"/>
+      <c r="G144" s="84"/>
+      <c r="H144" s="85"/>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145" s="27" t="s">
@@ -15041,15 +15037,15 @@
     </row>
     <row r="154" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="155" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="75" t="s">
+      <c r="B155" s="83" t="s">
         <v>268</v>
       </c>
-      <c r="C155" s="76"/>
-      <c r="D155" s="76"/>
-      <c r="E155" s="76"/>
-      <c r="F155" s="76"/>
-      <c r="G155" s="76"/>
-      <c r="H155" s="77"/>
+      <c r="C155" s="84"/>
+      <c r="D155" s="84"/>
+      <c r="E155" s="84"/>
+      <c r="F155" s="84"/>
+      <c r="G155" s="84"/>
+      <c r="H155" s="85"/>
     </row>
     <row r="156" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B156" s="22" t="s">
@@ -15220,15 +15216,15 @@
       </c>
     </row>
     <row r="166" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="81" t="s">
+      <c r="B166" s="102" t="s">
         <v>271</v>
       </c>
-      <c r="C166" s="81"/>
-      <c r="D166" s="81"/>
-      <c r="E166" s="81"/>
-      <c r="F166" s="81"/>
-      <c r="G166" s="81"/>
-      <c r="H166" s="81"/>
+      <c r="C166" s="102"/>
+      <c r="D166" s="102"/>
+      <c r="E166" s="102"/>
+      <c r="F166" s="102"/>
+      <c r="G166" s="102"/>
+      <c r="H166" s="102"/>
     </row>
     <row r="167" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B167" s="22" t="s">
@@ -15296,16 +15292,16 @@
       <c r="H169" s="3">
         <v>155</v>
       </c>
-      <c r="J169" s="82" t="s">
+      <c r="J169" s="93" t="s">
         <v>275</v>
       </c>
-      <c r="K169" s="83"/>
-      <c r="L169" s="83"/>
-      <c r="M169" s="83"/>
-      <c r="N169" s="83"/>
-      <c r="O169" s="83"/>
-      <c r="P169" s="83"/>
-      <c r="Q169" s="84"/>
+      <c r="K169" s="96"/>
+      <c r="L169" s="96"/>
+      <c r="M169" s="96"/>
+      <c r="N169" s="96"/>
+      <c r="O169" s="96"/>
+      <c r="P169" s="96"/>
+      <c r="Q169" s="97"/>
     </row>
     <row r="170" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B170" s="3">
@@ -15410,15 +15406,15 @@
     </row>
     <row r="175" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="176" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="85" t="s">
+      <c r="B176" s="90" t="s">
         <v>276</v>
       </c>
-      <c r="C176" s="86"/>
-      <c r="D176" s="86"/>
-      <c r="E176" s="86"/>
-      <c r="F176" s="86"/>
-      <c r="G176" s="86"/>
-      <c r="H176" s="87"/>
+      <c r="C176" s="91"/>
+      <c r="D176" s="91"/>
+      <c r="E176" s="91"/>
+      <c r="F176" s="91"/>
+      <c r="G176" s="91"/>
+      <c r="H176" s="92"/>
     </row>
     <row r="177" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B177" s="22" t="s">
@@ -15478,16 +15474,16 @@
       <c r="F179" s="3"/>
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
-      <c r="J179" s="82" t="s">
+      <c r="J179" s="93" t="s">
         <v>280</v>
       </c>
-      <c r="K179" s="83"/>
-      <c r="L179" s="83"/>
-      <c r="M179" s="83"/>
-      <c r="N179" s="83"/>
-      <c r="O179" s="83"/>
-      <c r="P179" s="83"/>
-      <c r="Q179" s="84"/>
+      <c r="K179" s="96"/>
+      <c r="L179" s="96"/>
+      <c r="M179" s="96"/>
+      <c r="N179" s="96"/>
+      <c r="O179" s="96"/>
+      <c r="P179" s="96"/>
+      <c r="Q179" s="97"/>
     </row>
     <row r="180" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B180" s="3">
@@ -15592,15 +15588,15 @@
     </row>
     <row r="186" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="187" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B187" s="75" t="s">
+      <c r="B187" s="83" t="s">
         <v>287</v>
       </c>
-      <c r="C187" s="76"/>
-      <c r="D187" s="76"/>
-      <c r="E187" s="76"/>
-      <c r="F187" s="76"/>
-      <c r="G187" s="76"/>
-      <c r="H187" s="77"/>
+      <c r="C187" s="84"/>
+      <c r="D187" s="84"/>
+      <c r="E187" s="84"/>
+      <c r="F187" s="84"/>
+      <c r="G187" s="84"/>
+      <c r="H187" s="85"/>
     </row>
     <row r="188" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B188" s="22" t="s">
@@ -15804,15 +15800,15 @@
     </row>
     <row r="199" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="200" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="75" t="s">
+      <c r="B200" s="83" t="s">
         <v>294</v>
       </c>
-      <c r="C200" s="76"/>
-      <c r="D200" s="76"/>
-      <c r="E200" s="76"/>
-      <c r="F200" s="76"/>
-      <c r="G200" s="76"/>
-      <c r="H200" s="77"/>
+      <c r="C200" s="84"/>
+      <c r="D200" s="84"/>
+      <c r="E200" s="84"/>
+      <c r="F200" s="84"/>
+      <c r="G200" s="84"/>
+      <c r="H200" s="85"/>
     </row>
     <row r="201" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B201" s="22" t="s">
@@ -16068,15 +16064,15 @@
     </row>
     <row r="214" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="215" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B215" s="75" t="s">
+      <c r="B215" s="83" t="s">
         <v>299</v>
       </c>
-      <c r="C215" s="76"/>
-      <c r="D215" s="76"/>
-      <c r="E215" s="76"/>
-      <c r="F215" s="76"/>
-      <c r="G215" s="76"/>
-      <c r="H215" s="77"/>
+      <c r="C215" s="84"/>
+      <c r="D215" s="84"/>
+      <c r="E215" s="84"/>
+      <c r="F215" s="84"/>
+      <c r="G215" s="84"/>
+      <c r="H215" s="85"/>
     </row>
     <row r="216" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B216" s="22" t="s">
@@ -16314,15 +16310,15 @@
     </row>
     <row r="229" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="230" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B230" s="75" t="s">
+      <c r="B230" s="83" t="s">
         <v>307</v>
       </c>
-      <c r="C230" s="76"/>
-      <c r="D230" s="76"/>
-      <c r="E230" s="76"/>
-      <c r="F230" s="76"/>
-      <c r="G230" s="76"/>
-      <c r="H230" s="77"/>
+      <c r="C230" s="84"/>
+      <c r="D230" s="84"/>
+      <c r="E230" s="84"/>
+      <c r="F230" s="84"/>
+      <c r="G230" s="84"/>
+      <c r="H230" s="85"/>
     </row>
     <row r="231" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B231" s="22" t="s">
@@ -16511,15 +16507,15 @@
     </row>
     <row r="241" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="242" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B242" s="75" t="s">
+      <c r="B242" s="83" t="s">
         <v>310</v>
       </c>
-      <c r="C242" s="76"/>
-      <c r="D242" s="76"/>
-      <c r="E242" s="76"/>
-      <c r="F242" s="76"/>
-      <c r="G242" s="76"/>
-      <c r="H242" s="77"/>
+      <c r="C242" s="84"/>
+      <c r="D242" s="84"/>
+      <c r="E242" s="84"/>
+      <c r="F242" s="84"/>
+      <c r="G242" s="84"/>
+      <c r="H242" s="85"/>
     </row>
     <row r="243" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B243" s="22" t="s">
@@ -16840,15 +16836,15 @@
     </row>
     <row r="259" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="260" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B260" s="75" t="s">
+      <c r="B260" s="83" t="s">
         <v>319</v>
       </c>
-      <c r="C260" s="76"/>
-      <c r="D260" s="76"/>
-      <c r="E260" s="76"/>
-      <c r="F260" s="76"/>
-      <c r="G260" s="76"/>
-      <c r="H260" s="77"/>
+      <c r="C260" s="84"/>
+      <c r="D260" s="84"/>
+      <c r="E260" s="84"/>
+      <c r="F260" s="84"/>
+      <c r="G260" s="84"/>
+      <c r="H260" s="85"/>
     </row>
     <row r="261" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B261" s="22" t="s">
@@ -17073,15 +17069,15 @@
     </row>
     <row r="273" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="274" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B274" s="75" t="s">
+      <c r="B274" s="83" t="s">
         <v>323</v>
       </c>
-      <c r="C274" s="76"/>
-      <c r="D274" s="76"/>
-      <c r="E274" s="76"/>
-      <c r="F274" s="76"/>
-      <c r="G274" s="76"/>
-      <c r="H274" s="77"/>
+      <c r="C274" s="84"/>
+      <c r="D274" s="84"/>
+      <c r="E274" s="84"/>
+      <c r="F274" s="84"/>
+      <c r="G274" s="84"/>
+      <c r="H274" s="85"/>
     </row>
     <row r="275" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B275" s="22" t="s">
@@ -17147,15 +17143,15 @@
         <v>184</v>
       </c>
       <c r="H277" s="35"/>
-      <c r="J277" s="78" t="s">
+      <c r="J277" s="101" t="s">
         <v>327</v>
       </c>
-      <c r="K277" s="79"/>
-      <c r="L277" s="79"/>
-      <c r="M277" s="79"/>
-      <c r="N277" s="79"/>
-      <c r="O277" s="79"/>
-      <c r="P277" s="80"/>
+      <c r="K277" s="94"/>
+      <c r="L277" s="94"/>
+      <c r="M277" s="94"/>
+      <c r="N277" s="94"/>
+      <c r="O277" s="94"/>
+      <c r="P277" s="95"/>
     </row>
     <row r="278" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B278" s="34">
@@ -17260,15 +17256,15 @@
     </row>
     <row r="284" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="285" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B285" s="75" t="s">
+      <c r="B285" s="83" t="s">
         <v>329</v>
       </c>
-      <c r="C285" s="76"/>
-      <c r="D285" s="76"/>
-      <c r="E285" s="76"/>
-      <c r="F285" s="76"/>
-      <c r="G285" s="76"/>
-      <c r="H285" s="77"/>
+      <c r="C285" s="84"/>
+      <c r="D285" s="84"/>
+      <c r="E285" s="84"/>
+      <c r="F285" s="84"/>
+      <c r="G285" s="84"/>
+      <c r="H285" s="85"/>
     </row>
     <row r="286" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B286" s="22" t="s">
@@ -17494,14 +17490,14 @@
       </c>
     </row>
     <row r="299" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B299" s="74" t="s">
+      <c r="B299" s="103" t="s">
         <v>194</v>
       </c>
-      <c r="C299" s="74"/>
-      <c r="D299" s="74"/>
-      <c r="E299" s="74"/>
-      <c r="F299" s="74"/>
-      <c r="G299" s="74"/>
+      <c r="C299" s="103"/>
+      <c r="D299" s="103"/>
+      <c r="E299" s="103"/>
+      <c r="F299" s="103"/>
+      <c r="G299" s="103"/>
     </row>
     <row r="300" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B300" s="11" t="s">
@@ -17666,15 +17662,15 @@
     </row>
     <row r="309" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="310" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B310" s="75" t="s">
+      <c r="B310" s="83" t="s">
         <v>333</v>
       </c>
-      <c r="C310" s="76"/>
-      <c r="D310" s="76"/>
-      <c r="E310" s="76"/>
-      <c r="F310" s="76"/>
-      <c r="G310" s="76"/>
-      <c r="H310" s="77"/>
+      <c r="C310" s="84"/>
+      <c r="D310" s="84"/>
+      <c r="E310" s="84"/>
+      <c r="F310" s="84"/>
+      <c r="G310" s="84"/>
+      <c r="H310" s="85"/>
     </row>
     <row r="311" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B311" s="22" t="s">
@@ -17872,6 +17868,24 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B299:G299"/>
+    <mergeCell ref="B310:H310"/>
+    <mergeCell ref="B285:H285"/>
+    <mergeCell ref="B230:H230"/>
+    <mergeCell ref="B242:H242"/>
+    <mergeCell ref="B260:H260"/>
+    <mergeCell ref="B274:H274"/>
+    <mergeCell ref="J277:P277"/>
+    <mergeCell ref="B144:H144"/>
+    <mergeCell ref="B133:H133"/>
+    <mergeCell ref="B187:H187"/>
+    <mergeCell ref="B200:H200"/>
+    <mergeCell ref="B215:H215"/>
+    <mergeCell ref="B155:H155"/>
+    <mergeCell ref="B166:H166"/>
+    <mergeCell ref="J169:Q169"/>
+    <mergeCell ref="B176:H176"/>
+    <mergeCell ref="J179:Q179"/>
     <mergeCell ref="B90:H90"/>
     <mergeCell ref="B106:H106"/>
     <mergeCell ref="B120:H120"/>
@@ -17887,24 +17901,6 @@
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B53:H53"/>
     <mergeCell ref="B65:H65"/>
-    <mergeCell ref="J277:P277"/>
-    <mergeCell ref="B144:H144"/>
-    <mergeCell ref="B133:H133"/>
-    <mergeCell ref="B187:H187"/>
-    <mergeCell ref="B200:H200"/>
-    <mergeCell ref="B215:H215"/>
-    <mergeCell ref="B155:H155"/>
-    <mergeCell ref="B166:H166"/>
-    <mergeCell ref="J169:Q169"/>
-    <mergeCell ref="B176:H176"/>
-    <mergeCell ref="J179:Q179"/>
-    <mergeCell ref="B299:G299"/>
-    <mergeCell ref="B310:H310"/>
-    <mergeCell ref="B285:H285"/>
-    <mergeCell ref="B230:H230"/>
-    <mergeCell ref="B242:H242"/>
-    <mergeCell ref="B260:H260"/>
-    <mergeCell ref="B274:H274"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>